<commit_message>
Updated np results based on updated criteria np
</commit_message>
<xml_diff>
--- a/results/accel-glmm-results/diel-period/np/glmm_ind_effects_dp_np.xlsx
+++ b/results/accel-glmm-results/diel-period/np/glmm_ind_effects_dp_np.xlsx
@@ -432,13 +432,13 @@
         <v>10</v>
       </c>
       <c r="E2" t="n">
-        <v>-1.81538175983053</v>
+        <v>-1.81538176693265</v>
       </c>
       <c r="F2" t="n">
-        <v>0.0316107915591497</v>
+        <v>0.0316107973062065</v>
       </c>
       <c r="G2" t="n">
-        <v>-57.4291775146984</v>
+        <v>-57.4291672983591</v>
       </c>
       <c r="H2" t="n">
         <v>0</v>
@@ -456,16 +456,16 @@
         <v>11</v>
       </c>
       <c r="E3" t="n">
-        <v>-0.0267036250185053</v>
+        <v>-0.0267036255433858</v>
       </c>
       <c r="F3" t="n">
-        <v>0.00726039246197363</v>
+        <v>0.00726039245976958</v>
       </c>
       <c r="G3" t="n">
-        <v>-3.67798643921327</v>
+        <v>-3.67798651262349</v>
       </c>
       <c r="H3" t="n">
-        <v>0.000235082454887743</v>
+        <v>0.000235082387245362</v>
       </c>
     </row>
     <row r="4">
@@ -480,16 +480,16 @@
         <v>12</v>
       </c>
       <c r="E4" t="n">
-        <v>0.0769598815389843</v>
+        <v>0.0769598821295752</v>
       </c>
       <c r="F4" t="n">
-        <v>0.00956265599382697</v>
+        <v>0.00956265598494264</v>
       </c>
       <c r="G4" t="n">
-        <v>8.04796090005377</v>
+        <v>8.04796096929099</v>
       </c>
       <c r="H4" t="n">
-        <v>0.00000000000000084184832492499</v>
+        <v>0.000000000000000841847848797373</v>
       </c>
     </row>
     <row r="5">
@@ -504,16 +504,16 @@
         <v>13</v>
       </c>
       <c r="E5" t="n">
-        <v>-0.127943282277576</v>
+        <v>-0.127943282302132</v>
       </c>
       <c r="F5" t="n">
-        <v>0.00724807346826162</v>
+        <v>0.00724807346545028</v>
       </c>
       <c r="G5" t="n">
-        <v>-17.6520399300342</v>
+        <v>-17.652039940269</v>
       </c>
       <c r="H5" t="n">
-        <v>0.000000000000000000000000000000000000000000000000000000000000000000000981461900160301</v>
+        <v>0.000000000000000000000000000000000000000000000000000000000000000000000981461722278886</v>
       </c>
     </row>
     <row r="6">
@@ -530,7 +530,7 @@
         <v>16</v>
       </c>
       <c r="E6" t="n">
-        <v>0.137093198611736</v>
+        <v>0.1370932252419</v>
       </c>
       <c r="F6"/>
       <c r="G6"/>

</xml_diff>